<commit_message>
CV ajustes en los módulos de productos
</commit_message>
<xml_diff>
--- a/FALEC-w1-core-web/WebContent/reportes/FALECPV-Inventario.xlsx
+++ b/FALEC-w1-core-web/WebContent/reportes/FALECPV-Inventario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/projects/gitrepositorio/FacturaElectronica-App/FALEC-w1-core-web/WebContent/reportes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33881071-0BD1-5C4F-8B83-C043462DD8B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD90162B-5619-2C4A-B937-E1FE9C588106}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1520" yWindow="7580" windowWidth="27640" windowHeight="16940" xr2:uid="{E9788733-D204-D84A-A824-443E01B2DF94}"/>
   </bookViews>
@@ -30,9 +30,6 @@
     <t>CODIGO</t>
   </si>
   <si>
-    <t>CATEGORIA</t>
-  </si>
-  <si>
     <t>FABRICANTE</t>
   </si>
   <si>
@@ -66,9 +63,6 @@
     <t>ESTABLECIMEINTO :</t>
   </si>
   <si>
-    <t xml:space="preserve">USURIO : </t>
-  </si>
-  <si>
     <t>FECHA :</t>
   </si>
   <si>
@@ -76,6 +70,12 @@
   </si>
   <si>
     <t>COSTO TOTAL :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USUARIO : </t>
+  </si>
+  <si>
+    <t>CATEGORÍA</t>
   </si>
 </sst>
 </file>
@@ -488,7 +488,7 @@
   <dimension ref="A2:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -507,7 +507,7 @@
   <sheetData>
     <row r="2" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -522,7 +522,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -530,7 +530,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -538,7 +538,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -546,47 +546,47 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CV errores de inventario en los reportes de inventario
</commit_message>
<xml_diff>
--- a/FALEC-w1-core-web/WebContent/reportes/FALECPV-Inventario.xlsx
+++ b/FALEC-w1-core-web/WebContent/reportes/FALECPV-Inventario.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10615"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/projects/gitrepositorio/FacturaElectronica-App/FALEC-w1-core-web/WebContent/reportes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD90162B-5619-2C4A-B937-E1FE9C588106}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1BE4943-923E-F64A-9862-6ECC91C35028}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1520" yWindow="7580" windowWidth="27640" windowHeight="16940" xr2:uid="{E9788733-D204-D84A-A824-443E01B2DF94}"/>
   </bookViews>
@@ -488,7 +488,7 @@
   <dimension ref="A2:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -583,10 +583,16 @@
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>14</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>